<commit_message>
Template with fill in instruction
</commit_message>
<xml_diff>
--- a/src/csv/empty template.xlsx
+++ b/src/csv/empty template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/itai/Documents/ourGovernment-React/src/csv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/itai/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206A01D0-F556-5F4D-AE6D-E2183B70E654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0321B972-EBC7-224A-8F9B-C94D782E8CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="1" xr2:uid="{31000AA0-AA0E-064D-83DB-D33034594433}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{31000AA0-AA0E-064D-83DB-D33034594433}"/>
   </bookViews>
   <sheets>
     <sheet name="Votes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -106,13 +106,187 @@
   </si>
   <si>
     <t>candidate #2.7</t>
+  </si>
+  <si>
+    <t>File fill instructions:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Offices:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+      </rPr>
+      <t xml:space="preserve">• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Fill in the names of the offices (it is not necessary to  
+  fill in all the columns)
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+      </rPr>
+      <t>Additional office columns can be added to the right of    
+  the table</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Candidates:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+      </rPr>
+      <t>• Fill in the names of the candidates for each office in 
+  the appropriate column (a different number of 
+  candidates can be defined for each office).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+• Additional candidate rows can be added to the bottom 
+  of the table
+• Note: Each candidate can apply for a position in only 
+  one office.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Votes:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+• To fill in the votes, go to 'Votes' sheet.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+      </rPr>
+      <t>First fill out the 'Offices &amp; Candidates' sheet.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Voter identity:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+• For each voter, write his or her ID under the ID column.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>How to vote:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+• Each voter must choose the preferred candidate for 
+  each ministry (it is possible not to choose a candidate 
+  for a particular ministry and this will be considered a 
+  "white note").
+</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,8 +315,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aharoni"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Nova Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Nova Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Nova Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Nova Light"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Nova Light"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,8 +372,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -326,11 +549,81 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -399,6 +692,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -410,6 +721,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,6 +737,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB2B2B2"/>
+      <color rgb="FF969696"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -440,8 +766,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>103248</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>44581</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1529998</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -488,9 +814,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1334331</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>1334330</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1426883</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -823,35 +1149,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251182A5-2D0A-3247-AD3A-7C97976E41D9}">
-  <dimension ref="C1:L42"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A3" zoomScale="112" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="18"/>
-    <col min="2" max="2" width="26.1640625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="41" style="18" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" style="18" customWidth="1"/>
     <col min="4" max="10" width="22.6640625" style="18" customWidth="1"/>
     <col min="11" max="14" width="22.83203125" style="18" customWidth="1"/>
     <col min="15" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="25"/>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="27"/>
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
     </row>
-    <row r="3" spans="3:12" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
@@ -861,7 +1197,7 @@
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="3:12" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="20" t="s">
         <v>2</v>
       </c>
@@ -875,7 +1211,7 @@
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
     </row>
-    <row r="5" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="16" t="s">
         <v>0</v>
       </c>
@@ -910,7 +1246,7 @@
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C6" s="14">
         <v>10</v>
       </c>
@@ -924,7 +1260,7 @@
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C7" s="14">
         <v>11</v>
       </c>
@@ -938,7 +1274,7 @@
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C8" s="14">
         <v>12</v>
       </c>
@@ -952,7 +1288,7 @@
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C9" s="14">
         <v>13</v>
       </c>
@@ -966,7 +1302,7 @@
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C10" s="14">
         <v>14</v>
       </c>
@@ -980,7 +1316,7 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C11" s="14">
         <v>15</v>
       </c>
@@ -994,7 +1330,7 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C12" s="14">
         <v>16</v>
       </c>
@@ -1008,7 +1344,7 @@
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C13" s="14">
         <v>17</v>
       </c>
@@ -1022,7 +1358,7 @@
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C14" s="14">
         <v>18</v>
       </c>
@@ -1036,7 +1372,7 @@
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C15" s="14">
         <v>19</v>
       </c>
@@ -1050,7 +1386,7 @@
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C16" s="14">
         <v>20</v>
       </c>
@@ -1283,12 +1619,15 @@
       <c r="L42" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
@@ -1342,15 +1681,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A91BC5-5470-A441-AE5A-8F8BE0C5F647}">
-  <dimension ref="C3:I12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="11"/>
+    <col min="1" max="1" width="10.83203125" style="11"/>
+    <col min="2" max="2" width="40" style="11" customWidth="1"/>
     <col min="3" max="3" width="23.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="11" bestFit="1" customWidth="1"/>
@@ -1361,23 +1701,37 @@
     <col min="10" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" ht="103" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-    </row>
-    <row r="4" spans="3:9" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="24" t="s">
+    <row r="1" spans="1:9" ht="22.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="35"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="27"/>
+    </row>
+    <row r="3" spans="1:9" ht="214" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1400,7 +1754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1413,7 +1767,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1426,7 +1780,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1439,7 +1793,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1452,7 +1806,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1465,7 +1819,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1478,7 +1832,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
         <v>16</v>
       </c>
@@ -1492,12 +1846,23 @@
       <c r="I12" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Duplicate office name" error="You wrote a duplicate office name" promptTitle="Office name" prompt="You must write a different office name for each office" sqref="C5:AR5" xr:uid="{08506122-1988-4546-84AC-E9B3AA862232}">
+      <formula1>COUNTIF($C$5:$AR$5,C5)=1</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Duplicate candidate name" error="You wrote a duplicate candidate name" promptTitle="Candidate name" prompt="You must write a different name for each candidate" sqref="C6:EH1372" xr:uid="{4F089228-1309-4C69-9EDF-1B7EBCEE5C8D}">
+      <formula1>COUNTIF($C$6:$EH$1372,C6)=1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>